<commit_message>
Adding new stats for barriers and data.csv
</commit_message>
<xml_diff>
--- a/ResearchSPSS/Excel and Charts/Odds Ratio.xlsx
+++ b/ResearchSPSS/Excel and Charts/Odds Ratio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameepshah/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameepshah/Documents/Research/ResearchWomensHealth/ResearchSPSS/Excel and Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF64739-475E-5244-B575-B9DABB9085E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF84626-6DD9-224E-8A5C-5CCDA73C3C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23320" xr2:uid="{09A2218C-6EE7-C14A-86DF-085EE69D4C72}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
   <si>
     <t>Mammogram</t>
   </si>
@@ -134,14 +134,49 @@
   </si>
   <si>
     <t>&lt;40k</t>
+  </si>
+  <si>
+    <t>No breast exam</t>
+  </si>
+  <si>
+    <t>Breast exam</t>
+  </si>
+  <si>
+    <t>NB/B</t>
+  </si>
+  <si>
+    <t>No BE</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>Barriers</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,8 +204,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC1B5EA-567E-8642-9587-1514E2E298AF}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,9 +535,10 @@
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -519,8 +557,17 @@
       <c r="K1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -553,8 +600,21 @@
         <f>L2/L5 %</f>
         <v>28.125</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>21</v>
+      </c>
+      <c r="S2">
+        <f>Q2/R2</f>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -587,8 +647,21 @@
         <f>L3/L5 %</f>
         <v>14.0625</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>12</v>
+      </c>
+      <c r="S3">
+        <f>Q3/R3</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K4" t="s">
         <v>28</v>
       </c>
@@ -600,7 +673,7 @@
         <v>57.8125</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -612,8 +685,15 @@
         <f>SUM(L2:L4)</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <f>S2/S3</f>
+        <v>5.7142857142857144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -629,8 +709,14 @@
       <c r="M7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -657,8 +743,21 @@
         <f>L8/M8</f>
         <v>3.6363636363636362</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <f>Q8/R8</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -685,8 +784,21 @@
         <f>L9/M9</f>
         <v>0.8571428571428571</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>11</v>
+      </c>
+      <c r="S9">
+        <f>Q9/R9</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -701,8 +813,15 @@
         <f>N8/N9</f>
         <v>4.2424242424242422</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R11" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <f>S8/S9</f>
+        <v>7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -712,8 +831,11 @@
       <c r="K13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -738,8 +860,14 @@
       <c r="M14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q14" t="s">
+        <v>36</v>
+      </c>
+      <c r="R14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -779,8 +907,21 @@
         <f>L15/M15</f>
         <v>4.125</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>27</v>
+      </c>
+      <c r="S15">
+        <f>Q15/R15</f>
+        <v>0.37037037037037035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -820,8 +961,21 @@
         <f>L16/M16</f>
         <v>1.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>19</v>
+      </c>
+      <c r="S16">
+        <f>Q16/R16</f>
+        <v>0.15789473684210525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -843,13 +997,20 @@
         <f>N15/N16</f>
         <v>3.1730769230769229</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <f>S15/S16</f>
+        <v>2.3456790123456792</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -874,8 +1035,14 @@
       <c r="M20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -915,8 +1082,21 @@
         <f>L21/M21</f>
         <v>2.8571428571428572</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P21" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+      <c r="R21">
+        <v>16</v>
+      </c>
+      <c r="S21">
+        <f>Q21/R21</f>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -956,8 +1136,21 @@
         <f>L22/M22</f>
         <v>2.3636363636363638</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>14</v>
+      </c>
+      <c r="S22">
+        <f>Q22/R22</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>4</v>
       </c>
@@ -979,16 +1172,32 @@
         <f>N21/N22</f>
         <v>1.2087912087912087</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R24" t="s">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <f>S21/S22</f>
+        <v>3.0625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" t="s">
+        <v>41</v>
+      </c>
+      <c r="P25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -1007,8 +1216,24 @@
       <c r="I26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>11</v>
+      </c>
+      <c r="M26">
+        <f>L26/48%</f>
+        <v>22.916666666666668</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1035,8 +1260,31 @@
         <f>G27/H27</f>
         <v>0.17647058823529413</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M31" si="0">L27/48%</f>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="P27" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q27">
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>16</v>
+      </c>
+      <c r="S27">
+        <f>Q27/R27</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1063,8 +1311,43 @@
         <f>G28/H28</f>
         <v>9.375E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>10.416666666666668</v>
+      </c>
+      <c r="P28" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q28">
+        <v>8</v>
+      </c>
+      <c r="R28">
+        <v>30</v>
+      </c>
+      <c r="S28">
+        <f>Q28/R28</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -1079,8 +1362,37 @@
         <f>I27/I28</f>
         <v>1.8823529411764708</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>19</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>39.583333333333336</v>
+      </c>
+      <c r="R30" t="s">
+        <v>4</v>
+      </c>
+      <c r="S30">
+        <f>S27/S28</f>
+        <v>1.171875</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>11</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>22.916666666666668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>5</v>
       </c>
@@ -1099,8 +1411,21 @@
       <c r="I32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32">
+        <f>SUM(L26:L31)</f>
+        <v>48</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1127,8 +1452,21 @@
         <f>G33/H33</f>
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="P33" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+      <c r="R33">
+        <v>7</v>
+      </c>
+      <c r="S33">
+        <f>Q33/R33</f>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1155,8 +1493,21 @@
         <f>G34/H34</f>
         <v>0.38095238095238093</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="P34" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34">
+        <v>4</v>
+      </c>
+      <c r="R34">
+        <v>23</v>
+      </c>
+      <c r="S34">
+        <f>Q34/R34</f>
+        <v>0.17391304347826086</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>4</v>
       </c>
@@ -1170,6 +1521,172 @@
       <c r="I36">
         <f>I33/I34</f>
         <v>1.5</v>
+      </c>
+      <c r="R36" t="s">
+        <v>4</v>
+      </c>
+      <c r="S36">
+        <f>S33/S34</f>
+        <v>4.1071428571428577</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <f>B39/B45 %</f>
+        <v>41.379310344827587</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>21</v>
+      </c>
+      <c r="H39">
+        <f>G39/52 %</f>
+        <v>40.38461538461538</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f>B40/B45%</f>
+        <v>6.8965517241379315</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:H44" si="1">G40/52 %</f>
+        <v>5.7692307692307692</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <f>B41/B45%</f>
+        <v>10.344827586206897</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>12</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <f>B42/B45%</f>
+        <v>3.4482758620689657</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <f>B43/B45%</f>
+        <v>17.241379310344829</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>9.615384615384615</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <f>B44/B45%</f>
+        <v>20.689655172413794</v>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>11</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>21.153846153846153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45">
+        <f>SUM(B39:B44)</f>
+        <v>29</v>
+      </c>
+      <c r="F45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45">
+        <f>SUM(G39:G44)</f>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>